<commit_message>
added functionality to infer significant mappings from the workbook itself
</commit_message>
<xml_diff>
--- a/auditing_automation/data/workbook_to_copy.xlsx
+++ b/auditing_automation/data/workbook_to_copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fosa/PythonProjects/git_tree/auditing_automation/xlwings_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fosa/PythonProjects/git_tree/auditing_automation/auditing_automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71E5555-928C-2C42-A1B5-C841C50DAB7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3686A016-64A7-1D48-986E-C73D0E610F6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="13900" xr2:uid="{6D501CA2-B23A-2B48-B2C2-E8CE2BD33026}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>GL Acct</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Subcategory</t>
   </si>
   <si>
-    <t>Input - Mapping</t>
-  </si>
-  <si>
     <t>Bank A</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Advance Payments from related party</t>
+  </si>
+  <si>
+    <t>Significant Mappings</t>
   </si>
 </sst>
 </file>
@@ -129,18 +129,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,12 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +470,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,291 +498,294 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>11923940590</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>11923940590</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>25</v>
       </c>
-      <c r="D2" s="3">
-        <v>39</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="2">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>11923940591</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>11923940591</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>11923940592</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="2">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>11923940593</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>11923940594</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>11923940595</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>11923940596</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>11923940597</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>11923940598</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>11923940599</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
         <v>26</v>
       </c>
-      <c r="D3" s="3">
-        <v>39</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>11923940592</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="D11" s="2">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11923940600</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2">
         <v>27</v>
       </c>
-      <c r="D4" s="3">
-        <v>39</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>11923940593</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="D12" s="2">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>11923940601</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2">
         <v>28</v>
       </c>
-      <c r="D5" s="3">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>11923940594</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="D13" s="2">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11923940602</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2">
         <v>29</v>
       </c>
-      <c r="D6" s="3">
-        <v>39</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>11923940595</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="D14" s="2">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>11923940603</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2">
         <v>30</v>
       </c>
-      <c r="D7" s="3">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>11923940596</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3">
-        <v>39</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>11923940597</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3">
-        <v>32</v>
-      </c>
-      <c r="D9" s="3">
-        <v>39</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>11923940598</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <v>39</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>11923940599</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3">
-        <v>39</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>11923940600</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3">
-        <v>39</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>11923940601</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="D15" s="2">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3">
-        <v>28</v>
-      </c>
-      <c r="D13" s="3">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>11923940602</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3">
-        <v>29</v>
-      </c>
-      <c r="D14" s="3">
-        <v>39</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>11923940603</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3">
-        <v>30</v>
-      </c>
-      <c r="D15" s="3">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>